<commit_message>
Offset imp. og test skrevet ind
</commit_message>
<xml_diff>
--- a/rapportAfsnit/eProblemloesning/Test/Målinger_Offset_Forstærker.xlsx
+++ b/rapportAfsnit/eProblemloesning/Test/Målinger_Offset_Forstærker.xlsx
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,10 +1711,10 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>32</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>32</v>
@@ -1754,10 +1754,10 @@
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
faktor 3 skrevet ind
</commit_message>
<xml_diff>
--- a/rapportAfsnit/eProblemloesning/Test/Målinger_Offset_Forstærker.xlsx
+++ b/rapportAfsnit/eProblemloesning/Test/Målinger_Offset_Forstærker.xlsx
@@ -204,15 +204,6 @@
     <t>1.3543V</t>
   </si>
   <si>
-    <t>\-0.000082V</t>
-  </si>
-  <si>
-    <t>\-0.000103V</t>
-  </si>
-  <si>
-    <t>\-0.000118V</t>
-  </si>
-  <si>
     <t>1.5902V</t>
   </si>
   <si>
@@ -280,6 +271,15 @@
   </si>
   <si>
     <t>4.8799V</t>
+  </si>
+  <si>
+    <t>\-0.0082V</t>
+  </si>
+  <si>
+    <t>\-0.0103V</t>
+  </si>
+  <si>
+    <t>\-0.00118V</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="H23" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1692,7 +1692,7 @@
         <v>47</v>
       </c>
       <c r="S10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.3">
@@ -1755,10 +1755,10 @@
         <v>32</v>
       </c>
       <c r="R13" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.3">
@@ -1771,10 +1771,10 @@
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.3">
       <c r="Q15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.3">
@@ -1800,7 +1800,7 @@
         <v>29</v>
       </c>
       <c r="S16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="10:21" x14ac:dyDescent="0.3">
@@ -1892,13 +1892,13 @@
         <v>34</v>
       </c>
       <c r="S20" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="T20" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="U20" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="10:21" x14ac:dyDescent="0.3">
@@ -1915,13 +1915,13 @@
         <v>57</v>
       </c>
       <c r="S21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="T21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="U21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="10:21" x14ac:dyDescent="0.3">
@@ -1934,7 +1934,7 @@
     </row>
     <row r="26" spans="10:21" x14ac:dyDescent="0.3">
       <c r="Q26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="10:21" x14ac:dyDescent="0.3">
@@ -1953,7 +1953,7 @@
         <v>47</v>
       </c>
       <c r="S28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="10:21" x14ac:dyDescent="0.3">
@@ -1972,23 +1972,23 @@
         <v>32</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="S31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="17:21" x14ac:dyDescent="0.3">
       <c r="Q33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S33" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="34" spans="17:21" x14ac:dyDescent="0.3">
       <c r="S34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="17:21" x14ac:dyDescent="0.3">
@@ -2013,16 +2013,16 @@
         <v>32</v>
       </c>
       <c r="R37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="S37" t="s">
+        <v>74</v>
+      </c>
+      <c r="T37" t="s">
+        <v>76</v>
+      </c>
+      <c r="U37" t="s">
         <v>77</v>
-      </c>
-      <c r="T37" t="s">
-        <v>79</v>
-      </c>
-      <c r="U37" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="17:21" x14ac:dyDescent="0.3">
@@ -2038,7 +2038,7 @@
     </row>
     <row r="42" spans="17:21" x14ac:dyDescent="0.3">
       <c r="Q42" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="17:21" x14ac:dyDescent="0.3">
@@ -2063,16 +2063,16 @@
         <v>32</v>
       </c>
       <c r="R44" t="s">
+        <v>80</v>
+      </c>
+      <c r="S44" t="s">
+        <v>81</v>
+      </c>
+      <c r="T44" t="s">
+        <v>82</v>
+      </c>
+      <c r="U44" t="s">
         <v>83</v>
-      </c>
-      <c r="S44" t="s">
-        <v>84</v>
-      </c>
-      <c r="T44" t="s">
-        <v>85</v>
-      </c>
-      <c r="U44" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="45" spans="17:21" x14ac:dyDescent="0.3">

</xml_diff>